<commit_message>
Latest version of RMSE Logic pushed
</commit_message>
<xml_diff>
--- a/Mechanisms/Four_Bar_Slider/TeachingLab_Slider_Crank/RMSE_Results/E/AngVel/f12RPM/RMSE.xlsx
+++ b/Mechanisms/Four_Bar_Slider/TeachingLab_Slider_Crank/RMSE_Results/E/AngVel/f12RPM/RMSE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adg66\Downloads\PMKS_Simulator_Verification\Mechanisms\Four_Bar_Slider\TeachingLab_Slider_Crank\RMSE_Results\E\AngVel\f12RPM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD89ACCB-3022-4115-92F8-748CCADECAC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3220637-D53A-41E9-876F-2FB05B2F0A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="16200" windowHeight="9308" xr2:uid="{C6B8D768-BB29-40E4-84C7-D543978BEA0E}"/>
+    <workbookView xWindow="1837" yWindow="1837" windowWidth="16201" windowHeight="9308" xr2:uid="{FE05CB4C-EDCC-4324-8311-9388328618A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -401,7 +401,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C1CDE8E-695D-4A8D-AA8B-64ADA409E77F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F41DA9AE-89C0-40E3-BF60-44A13FD2E731}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -410,7 +410,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1">
-        <v>21.413916904560562</v>
+        <v>21.065836791897731</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RMSE now works for crankslider
</commit_message>
<xml_diff>
--- a/Mechanisms/Four_Bar_Slider/TeachingLab_Slider_Crank/RMSE_Results/E/AngVel/f12RPM/RMSE.xlsx
+++ b/Mechanisms/Four_Bar_Slider/TeachingLab_Slider_Crank/RMSE_Results/E/AngVel/f12RPM/RMSE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adg66\Downloads\PMKS_Simulator_Verification\Mechanisms\Four_Bar_Slider\TeachingLab_Slider_Crank\RMSE_Results\E\AngVel\f12RPM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898C9B09-ADB1-4AC2-A00D-DD15E717862B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23EDB5AD-2792-43D9-BC84-C84B27CC1B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1837" yWindow="1837" windowWidth="16201" windowHeight="9308" xr2:uid="{FE05CB4C-EDCC-4324-8311-9388328618A7}"/>
+    <workbookView xWindow="1837" yWindow="1837" windowWidth="16201" windowHeight="9308" xr2:uid="{C4840E96-4D7F-44E6-8CDD-EDB200A468D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -401,7 +401,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F41DA9AE-89C0-40E3-BF60-44A13FD2E731}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AF4A6BC-2D3C-460F-8BE9-A759150CFC5B}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -410,7 +410,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1">
-        <v>21.065836791897731</v>
+        <v>0.23286633171732421</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjusted RMSE for 4-bar and Crank-slider. Angle and AngVel for WitMotion appear correctly. AngVel for Crank-slider also appear correctly. Need to verify 4-bar for WitMotion
</commit_message>
<xml_diff>
--- a/Mechanisms/Four_Bar_Slider/TeachingLab_Slider_Crank/RMSE_Results/E/AngVel/f12RPM/RMSE.xlsx
+++ b/Mechanisms/Four_Bar_Slider/TeachingLab_Slider_Crank/RMSE_Results/E/AngVel/f12RPM/RMSE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adg66\Downloads\PMKS_Simulator_Verification\Mechanisms\Four_Bar_Slider\TeachingLab_Slider_Crank\RMSE_Results\E\AngVel\f12RPM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adg66\Downloads\PMKS_Verification\Mechanisms\Four_Bar_Slider\TeachingLab_Slider_Crank\RMSE_Results\E\AngVel\f12RPM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7EEB12-629E-4F2F-BE00-448F74DCE573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0B59D5-0EE1-4DA0-8932-97BF85950FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1853" yWindow="1853" windowWidth="12509" windowHeight="6239" xr2:uid="{BFA0F68F-A6B3-4E48-A354-24A4E6A25B95}"/>
+    <workbookView xWindow="5040" yWindow="240" windowWidth="15120" windowHeight="8604" xr2:uid="{C3D36FA0-3F03-47AC-AEE9-D8277BA16A78}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -401,16 +401,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B984AD7C-AAA9-4F34-852C-D6869E423F8A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09CC2625-BC68-4ADB-A2B8-8E337994AD23}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>9.0944233193535853E-2</v>
+        <v>0.22833669819734606</v>
       </c>
     </row>
   </sheetData>

</xml_diff>